<commit_message>
fix problem with database
</commit_message>
<xml_diff>
--- a/workflows/genome-assembly/bacterial-genomic-short-reads-assembly/test-data/staramr_excel_report.xlsx
+++ b/workflows/genome-assembly/bacterial-genomic-short-reads-assembly/test-data/staramr_excel_report.xlsx
@@ -375,19 +375,19 @@
     <t>resfinder_gene_drug_version</t>
   </si>
   <si>
-    <t>/shared/ifbstor1/galaxy/mutable-data/dependencies/_conda/envs/mulled-v1-50d167472d35f4b3d40c0e43369adafb301df8a06c0471a38dc9a39220c30ff7/bin/staramr search --nprocs 1 --genome-size-lower-bound 4000000 --genome-size-upper-bound 6000000 --minimum-N50-value 10000 --minimum-contig-length 300 --unacceptable-number-contigs 1000 --pid-threshold 98.0 --percent-length-overlap-resfinder 60.0 --percent-length-overlap-plasmidfinder 60.0 --percent-length-overlap-pointfinder 95.0 --output-summary /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_ed011ea8-969d-456d-84b8-175be8a83c5b.dat --output-detailed-summary /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_58166d14-b8cf-4be8-9129-9a26848aaab1.dat --output-resfinder /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_0dfb63d8-9eb5-42a7-9028-acc2f68405c7.dat --output-plasmidfinder /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_2bfc2787-2ae8-4eed-af84-2505418cca41.dat --output-settings /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_f53cdfa2-c70b-4d94-b403-e1c781d7fd43.dat --output-excel results.xlsx --output-mlst /shared/ifbstor1/galaxy/jobs/003/833/3833096/outputs/dataset_69435455-5947-4d72-bf32-7c57deeecee5.dat --output-hits-dir staramr_hits shovill_contigs_fasta.fasta</t>
+    <t>/shared/ifbstor1/galaxy/mutable-data/dependencies/_conda/envs/mulled-v1-50d167472d35f4b3d40c0e43369adafb301df8a06c0471a38dc9a39220c30ff7/bin/staramr search --nprocs 1 --genome-size-lower-bound 4000000 --genome-size-upper-bound 6000000 --minimum-N50-value 10000 --minimum-contig-length 300 --unacceptable-number-contigs 1000 --pid-threshold 98.0 --percent-length-overlap-resfinder 60.0 --percent-length-overlap-plasmidfinder 60.0 --percent-length-overlap-pointfinder 95.0 --output-summary /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_93d66200-ea55-4dff-a489-8c02d9212aa7.dat --output-detailed-summary /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_df1ae156-84f5-453d-b381-acaf3ffbcf69.dat --output-resfinder /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_45578c87-faf5-49d4-a841-e6e71f81296c.dat --output-plasmidfinder /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_3049e167-768d-4d80-bba5-9aeb1c569a8b.dat --output-settings /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_acb5634f-be75-4cc0-9204-7728ecc14a4e.dat --output-excel results.xlsx --output-mlst /shared/ifbstor1/galaxy/jobs/003/856/3856697/outputs/galaxy_dataset_92c71ffa-2402-4439-950c-ec3b2d98f435.dat --output-hits-dir staramr_hits shovill_contigs_fasta.fasta</t>
   </si>
   <si>
     <t>0.10.0</t>
   </si>
   <si>
-    <t>2024-01-17 11:41:20</t>
-  </si>
-  <si>
-    <t>2024-01-17 11:41:46</t>
-  </si>
-  <si>
-    <t>0.43</t>
+    <t>2024-01-25 12:10:23</t>
+  </si>
+  <si>
+    <t>2024-01-25 12:14:49</t>
+  </si>
+  <si>
+    <t>4.43</t>
   </si>
   <si>
     <t>/shared/ifbstor1/galaxy/mutable-data/dependencies/_conda/envs/mulled-v1-50d167472d35f4b3d40c0e43369adafb301df8a06c0471a38dc9a39220c30ff7/lib/python3.11/site-packages/staramr/databases/data/dist/resfinder</t>

</xml_diff>